<commit_message>
added valueset for sonmed myelodysplastic diseases
</commit_message>
<xml_diff>
--- a/docs/ValueSet-hematopoietic-disorder-valueset.xlsx
+++ b/docs/ValueSet-hematopoietic-disorder-valueset.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-08-10T12:44:20-05:00</t>
+    <t>2022-08-10T13:05:09-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -99,7 +99,7 @@
     <t>is-a</t>
   </si>
   <si>
-    <t>414027002</t>
+    <t>109995007</t>
   </si>
   <si>
     <t/>

</xml_diff>